<commit_message>
Remove callback urls for initiateCaseDraft
</commit_message>
<xml_diff>
--- a/definitions/xlsx/ccd-config-base.xlsx
+++ b/definitions/xlsx/ccd-config-base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E685CB4-07AE-46F8-ABB4-879E5A1E6639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAEA6A0-E788-4D45-B8CB-6BBA4FFEC350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="3" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15077" uniqueCount="3197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15075" uniqueCount="3197">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -24392,7 +24392,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -36188,8 +36188,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -36398,12 +36398,7 @@
       <c r="G5" t="s">
         <v>1119</v>
       </c>
-      <c r="I5" t="s">
-        <v>1251</v>
-      </c>
-      <c r="J5" s="167" t="s">
-        <v>1252</v>
-      </c>
+      <c r="J5" s="167"/>
       <c r="K5" s="57"/>
       <c r="L5" s="57" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Remove callback urls for initiateCaseDraft (#39)
</commit_message>
<xml_diff>
--- a/definitions/xlsx/ccd-config-base.xlsx
+++ b/definitions/xlsx/ccd-config-base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E685CB4-07AE-46F8-ABB4-879E5A1E6639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAEA6A0-E788-4D45-B8CB-6BBA4FFEC350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="3" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15077" uniqueCount="3197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15075" uniqueCount="3197">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -24392,7 +24392,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -36188,8 +36188,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:XFD57"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -36398,12 +36398,7 @@
       <c r="G5" t="s">
         <v>1119</v>
       </c>
-      <c r="I5" t="s">
-        <v>1251</v>
-      </c>
-      <c r="J5" s="167" t="s">
-        <v>1252</v>
-      </c>
+      <c r="J5" s="167"/>
       <c r="K5" s="57"/>
       <c r="L5" s="57" t="s">
         <v>31</v>

</xml_diff>